<commit_message>
Update-Inprocess return to SD
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/RMRegisterTagTemplate.xlsx
+++ b/bin/Debug/Template/RMRegisterTagTemplate.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15808912-9F56-4760-BBA4-3BEB3A1A616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE1099E4-C308-46B9-AF5D-00FC720DF5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B55643B-660D-486C-B673-E46BBE604A86}"/>
+    <workbookView xWindow="8745" yWindow="4050" windowWidth="21600" windowHeight="8670" xr2:uid="{2B55643B-660D-486C-B673-E46BBE604A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Wire" sheetId="2" r:id="rId1"/>
-    <sheet name="Terminal" sheetId="3" r:id="rId2"/>
+    <sheet name="Terminal" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Pcs</t>
+  </si>
+  <si>
+    <t>ចំនួនក្បាលគៀបមុនពេលដើរ</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +115,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Khmer OS Battambang"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -215,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -260,6 +269,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -671,7 +683,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38E47D28-E055-42DB-8EFC-B2F21B072303}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42D79FB0-6642-456C-BEA8-93E34FC86065}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -742,7 +754,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDA45147-7458-4621-8A14-2E6BC0B983A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76637866-CF60-4767-8E78-5C766C9816A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1105,7 +1117,7 @@
       <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,35 +1131,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1184,26 +1196,26 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1219,7 +1231,7 @@
       <c r="F7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1292,53 +1304,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EA0E80-AC21-4374-A6AF-6997BA6157A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C56BC1-00FB-41EE-AC57-0E2DD2FF0E93}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="2" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+    <row r="1" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1347,10 +1356,9 @@
         <v>15</v>
       </c>
       <c r="D4" s="10"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1359,15 +1367,12 @@
       <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="D5" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
       <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1377,74 +1382,64 @@
       <c r="D6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="19"/>
-    </row>
-    <row r="7" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B3:E3"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.05" footer="0.05"/>
-  <pageSetup paperSize="70" scale="81" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="70" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update-RM Register Excel template
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/RMRegisterTagTemplate.xlsx
+++ b/bin/Debug/Template/RMRegisterTagTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE1099E4-C308-46B9-AF5D-00FC720DF5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232415AD-870D-46EE-BA18-0F1D0486B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="4050" windowWidth="21600" windowHeight="8670" xr2:uid="{2B55643B-660D-486C-B673-E46BBE604A86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B55643B-660D-486C-B673-E46BBE604A86}"/>
   </bookViews>
   <sheets>
     <sheet name="Wire" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>ចំនួនក្បាលគៀបមុនពេលដើរ</t>
+  </si>
+  <si>
+    <t>RM Code</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -274,9 +277,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,6 +285,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -331,8 +340,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="838200" y="845820"/>
-          <a:ext cx="99060" cy="232410"/>
+          <a:off x="838200" y="843182"/>
+          <a:ext cx="96422" cy="232410"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -617,6 +626,77 @@
         <a:xfrm>
           <a:off x="3760470" y="1379220"/>
           <a:ext cx="99060" cy="232410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>625720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>84699</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9775C8A2-42F3-7C04-CAE0-7EEA81BB6425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2318239" y="843182"/>
+          <a:ext cx="96422" cy="232410"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -764,6 +844,77 @@
         <a:xfrm>
           <a:off x="838200" y="1114425"/>
           <a:ext cx="97155" cy="232410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{138949F7-965B-4DD3-BAA4-2653CD8E8B9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="849499"/>
+          <a:ext cx="99454" cy="232410"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1117,7 +1268,7 @@
       <pane xSplit="7" ySplit="7" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" sqref="A1:G1"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,35 +1282,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -1196,26 +1349,26 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1231,7 +1384,7 @@
       <c r="F7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -1289,13 +1442,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B3:G3"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="G6:G7"/>
+    <mergeCell ref="D3:G3"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.05" footer="0.05"/>
   <pageSetup paperSize="70" scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1311,11 +1464,11 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,26 +1479,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1358,7 +1513,7 @@
       <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1372,7 +1527,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1432,10 +1587,9 @@
       <c r="D14" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:D3"/>
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.05" footer="0.05"/>

</xml_diff>